<commit_message>
correct column names used in workbook 2020
</commit_message>
<xml_diff>
--- a/coefficients/2019/01 Example Excel Book.xlsx
+++ b/coefficients/2019/01 Example Excel Book.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keithrichards/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinsmith/Projects/Other/qcdr/coefficients/2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F955C770-07F6-434B-B209-F5E9B93A8554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C8FF8E-B969-084F-9404-8BBBAF5D7A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12240" yWindow="460" windowWidth="35820" windowHeight="22460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="500" windowWidth="35820" windowHeight="22460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example Calculation" sheetId="1" r:id="rId1"/>
@@ -290,34 +290,34 @@
     <t>(365,Inf]</t>
   </si>
   <si>
-    <t>MDQ PRO (IROMS 17)</t>
+    <t>ODI.prob.mcd</t>
   </si>
   <si>
-    <t>MDQ PAIN NPRS (IROMS 18)</t>
+    <t>ODI.prob.pain</t>
   </si>
   <si>
-    <t>NDI PRO (IROMS 15)</t>
+    <t>NECK.prob.mcd</t>
   </si>
   <si>
-    <t>NDI PAIN NPRS (IROMS16) </t>
+    <t>NECK.prob.pain</t>
   </si>
   <si>
-    <t>KOS PRO (IROMS 11)</t>
+    <t>KNEE.prob.mcd</t>
   </si>
   <si>
-    <t>KOS PAIN NPRS (IROMS 12)</t>
+    <t>KNEE.prob.pain</t>
   </si>
   <si>
-    <t>LEFS PRO (IROMS 13 )</t>
+    <t>LEFS.prob.mcd</t>
   </si>
   <si>
-    <t>LEFS PAIN NPRS  (IROMS 14)</t>
+    <t>LEFS.prob.pain</t>
   </si>
   <si>
-    <t>DASH PRO (IROMS 19)</t>
+    <t>DASH.prob.mcd</t>
   </si>
   <si>
-    <t>DASH PAIN NPRS (IROMS 20) </t>
+    <t>DASH.prob.pain</t>
   </si>
 </sst>
 </file>
@@ -338,7 +338,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1628,11 +1627,11 @@
     <row r="29" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J29" t="str">
         <f>VLOOKUP("id", Intercepts!A1:L1, $P$1, FALSE)</f>
-        <v>MDQ PRO (IROMS 17)</v>
+        <v>ODI.prob.mcd</v>
       </c>
       <c r="L29" t="str">
         <f>VLOOKUP("id", Intercepts!$A1:$L1, $P$1, FALSE)</f>
-        <v>MDQ PRO (IROMS 17)</v>
+        <v>ODI.prob.mcd</v>
       </c>
       <c r="O29" t="s">
         <v>57</v>
@@ -2639,8 +2638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3726,8 +3725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17400,7 +17399,7 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D1" sqref="D1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>